<commit_message>
se crean nueva clase para la ejecucion de la limpieza de lineas
</commit_message>
<xml_diff>
--- a/build/resources/test/config_access/data.xlsx
+++ b/build/resources/test/config_access/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\src\test\resources\config_access\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EACF2B-E071-4425-A03A-0D116ED87D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4078918F-2E27-4E93-B788-3E769C658422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>MSIDN</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>3016876877</t>
+  </si>
+  <si>
+    <t>MSI</t>
+  </si>
+  <si>
+    <t>732111198172294</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -670,7 +676,9 @@
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -688,7 +696,9 @@
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -706,6 +716,9 @@
       <c r="C12" s="1">
         <v>3016876876</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
@@ -717,6 +730,9 @@
       <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
@@ -727,6 +743,9 @@
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit funcional de ejecucion bd y soap
</commit_message>
<xml_diff>
--- a/build/resources/test/config_access/data.xlsx
+++ b/build/resources/test/config_access/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>MSIDN</t>
   </si>
@@ -47,9 +47,6 @@
     <t>URL GATEWAYCBS</t>
   </si>
   <si>
-    <t>URL GATEWAY MG</t>
-  </si>
-  <si>
     <t>http://10.69.60.77:8180/tigo-pos-web/</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>service</t>
   </si>
   <si>
-    <t>http://10.65.45.12:9001/gatewaymgint/GatewayMGWSInt</t>
-  </si>
-  <si>
     <t>732111198172293</t>
   </si>
   <si>
@@ -125,17 +119,53 @@
     <t>3016876877</t>
   </si>
   <si>
-    <t>MSI</t>
+    <t>IMSI</t>
   </si>
   <si>
     <t>732111198172294</t>
+  </si>
+  <si>
+    <t>8957732111198172293</t>
+  </si>
+  <si>
+    <t>8957732111198172291</t>
+  </si>
+  <si>
+    <t>8957732111198172290</t>
+  </si>
+  <si>
+    <t>8957732111198172295</t>
+  </si>
+  <si>
+    <t>8957732111198172296</t>
+  </si>
+  <si>
+    <t>3016876873</t>
+  </si>
+  <si>
+    <t>3016877414</t>
+  </si>
+  <si>
+    <t>3016876878</t>
+  </si>
+  <si>
+    <t>732111198172295</t>
+  </si>
+  <si>
+    <t>732111198172296</t>
+  </si>
+  <si>
+    <t>732111198172297</t>
+  </si>
+  <si>
+    <t>732111198172299</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,14 +195,6 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -195,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -212,7 +234,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -528,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -540,14 +561,10 @@
     <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="38.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.54296875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="1"/>
+    <col min="5" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -560,121 +577,101 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:10">
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="7"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -685,87 +682,127 @@
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>3003324</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>3003324</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1">
         <v>3016876876</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>3003324</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>3003324</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" s="8"/>
+      <c r="D14" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>3003324</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>3003324</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>3003324</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>3003324</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>